<commit_message>
contraints completas y generar excels de salida
</commit_message>
<xml_diff>
--- a/src/main/resources/contestants.xlsx
+++ b/src/main/resources/contestants.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,29 +20,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="140">
   <si>
     <t xml:space="preserve">ID per jurat</t>
   </si>
   <si>
-    <t xml:space="preserve">Title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Names</t>
+    <t xml:space="preserve">Títol</t>
   </si>
   <si>
     <t xml:space="preserve">Centre</t>
   </si>
   <si>
-    <t xml:space="preserve">Topic</t>
+    <t xml:space="preserve">Modalitat</t>
   </si>
   <si>
     <t xml:space="preserve">Com veu el cervell? La percepció visual</t>
   </si>
   <si>
-    <t xml:space="preserve">Sara, Joan</t>
-  </si>
-  <si>
     <t xml:space="preserve">Escola Pàlcam</t>
   </si>
   <si>
@@ -70,9 +64,6 @@
     <t xml:space="preserve">'L''autoestima en l''adolescència'</t>
   </si>
   <si>
-    <t xml:space="preserve">Teresa Blanco</t>
-  </si>
-  <si>
     <t xml:space="preserve">Institut de Vilanova del Vallès</t>
   </si>
   <si>
@@ -82,21 +73,18 @@
     <t xml:space="preserve">Estudio sobre la ventilación en el entorno escolar</t>
   </si>
   <si>
-    <t xml:space="preserve">Miquel Ares</t>
-  </si>
-  <si>
     <t xml:space="preserve">IES Padre Luis Coloma</t>
   </si>
   <si>
     <t xml:space="preserve">'"Radiació ultraviolada: Anàlisi de l''exposició directa  reflectida i protecció ocular"'</t>
   </si>
   <si>
+    <t xml:space="preserve">sin nombre1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ciències pures</t>
   </si>
   <si>
-    <t xml:space="preserve">EL ORIGEN DE LA ARENA DE NUESTRAS PLAYAS</t>
-  </si>
-  <si>
     <t xml:space="preserve">COL·LEGI SANTA MARIA</t>
   </si>
   <si>
@@ -196,6 +184,9 @@
     <t xml:space="preserve">STEM &amp; Sphero: la robòtica a biologia propostes innovadores</t>
   </si>
   <si>
+    <t xml:space="preserve">sin nombre2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Positiu o negatiu? La pandèmia i els infants</t>
   </si>
   <si>
@@ -217,6 +208,9 @@
     <t xml:space="preserve">La nanomedicina contra el càncer no és el futur  és “avui”</t>
   </si>
   <si>
+    <t xml:space="preserve">sin nombre3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ciència té nom de dona: estudi del reconeixement del paper de les dones a la ciència</t>
   </si>
   <si>
@@ -268,15 +262,31 @@
     <t xml:space="preserve">A la caza de exoplanetas. Análisis de los tránsitos de WASP-12b</t>
   </si>
   <si>
-    <t xml:space="preserve">IES Margarita Salas,Ciències pures
-41,Leonardo da Vinci i alguns dels seus invents,Escola Mare de Déu de la Salut,Tecnologia
-42,Què amaguen els somnis?,Institut Carles Vallbona,Salut
-43,Desenvolupament de videojocs en 16-bits,Institut Joan Brudieu,Tecnologia
-44,'"ESTUDIO COMPARATIVO DE LA RESISTENCIA DE CINCO ACEITES (ACEITE DE OLIVA VIRGEN EXTRA,  ACEITE DE OLIVA VIRGEN, ACEITE DE GIRASOL VIRGEN, ACEITE DE GIRASOL ALTO OLEICO SIN REFINAR, ACEITE DE SÉSAMO) A SU REUTILIZACIÓN"',,Ciències pures
-45,"Un recorregut virtual per La Tèrmica (Roca Umbert Granollers): gaudeix-la!</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
+    <t xml:space="preserve">IES Margarita Salas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leonardo da Vinci i alguns dels seus invents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Què amaguen els somnis?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desenvolupament de videojocs en 16-bits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Institut Joan Brudieu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'"ESTUDIO COMPARATIVO DE LA RESISTENCIA DE CINCO ACEITES (ACEITE DE OLIVA VIRGEN EXTRA ACEITE DE OLIVA VIRGEN ACEITE DE GIRASOL VIRGEN ACEITE DE GIRASOL ALTO OLEICO SIN REFINAR ACEITE DE SÉSAMO) A SU REUTILIZACIÓN"'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ins.sin nombre1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un recorregut virtual per La Tèrmica (Roca Umbert Granollers): gaudeix-la!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ins.sin nombre2</t>
   </si>
   <si>
     <t xml:space="preserve">Cámara de Niebla Low Cost</t>
@@ -375,14 +385,28 @@
     <t xml:space="preserve">La cara oculta de la indústria de la moda: fast fashion i slow fashion</t>
   </si>
   <si>
-    <t xml:space="preserve">EASD Llotja,Art | Música | Pensament
-66,La física de l’espagueti: estudi del seu trencament aplicant peses,Institut Carles Vallbona,Ciències pures
-67,Bacteris superresistents. És la llum ultraviolada realment una aliada?,Institut Vilanova del Vallès,Naturals | Medi ambient
-68,'"AVALUACIÓ I COMPARACIÓ DE L''EFECTIVITAT I SEGURETAT DEL TRASPLANTAMENT DE MICROBIOTA FECAL: ANTIINFLAMATORIS I BIOLÒGICS PER AL TRACTAMENT DE LA MALALTIA INFLAMATÒRIA INTESTINAL"',,Salut
-69,"WScientifics. Rompiendo con el efecto Matilda. Una propuesta de ciencia igualdad e inclusión.</t>
+    <t xml:space="preserve">La física de l’espagueti: estudi del seu trencament aplicant peses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bacteris superresistents. És la llum ultraviolada realment una aliada?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'"AVALUACIÓ I COMPARACIÓ DE L''EFECTIVITAT I SEGURETAT DEL TRASPLANTAMENT DE MICROBIOTA FECAL: ANTIINFLAMATORIS I BIOLÒGICS PER AL TRACTAMENT DE LA MALALTIA INFLAMATÒRIA INTESTINAL"'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sin nombre4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WScientifics. Rompiendo con el efecto Matilda. Una propuesta de ciencia igualdad e inclusión.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ins.sin nombre3 </t>
   </si>
   <si>
     <t xml:space="preserve">ATTIC: CREACIÓ I PRODUCCIÓ D’UN EP MUSICAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ins.sin nombre4</t>
   </si>
   <si>
     <t xml:space="preserve">'Rehabilitació del Vapor Casanovas per a la instauració d''un coworking'</t>
@@ -430,7 +454,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -496,7 +519,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -516,18 +539,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F69"/>
+  <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D42" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E61" activeCellId="0" sqref="E61"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="124.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="65.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="44.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="101.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="44.55"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -543,25 +566,19 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -569,13 +586,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>9</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -583,13 +600,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -597,16 +614,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -614,16 +628,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -631,10 +642,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -642,13 +656,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>24</v>
+        <v>19</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -656,13 +670,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>26</v>
+        <v>22</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -670,13 +684,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -684,13 +698,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>30</v>
+        <v>26</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>27</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -698,13 +712,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>29</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -712,13 +726,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>34</v>
+        <v>30</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>31</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -726,13 +740,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>36</v>
+        <v>32</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>33</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -740,13 +754,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>38</v>
+        <v>34</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>35</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -754,13 +768,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>40</v>
+        <v>36</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>37</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -768,13 +782,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>39</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -782,13 +796,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>44</v>
+        <v>40</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -796,13 +810,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>46</v>
+        <v>42</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>43</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -810,13 +824,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>48</v>
+        <v>44</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -824,13 +838,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>49</v>
+        <v>45</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>46</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -838,13 +852,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>51</v>
+        <v>47</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>48</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -852,13 +866,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>53</v>
+        <v>49</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>50</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -866,13 +880,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>55</v>
+        <v>51</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>52</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -880,10 +894,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>14</v>
+        <v>53</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -891,13 +908,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>58</v>
+        <v>55</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>56</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -905,13 +922,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>60</v>
+        <v>57</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>58</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -919,13 +936,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>62</v>
+        <v>59</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -933,10 +950,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>8</v>
+        <v>61</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -944,13 +964,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>65</v>
+        <v>63</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -958,13 +978,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>66</v>
+        <v>64</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>39</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -972,13 +992,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -986,13 +1006,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>67</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1000,13 +1020,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>70</v>
+        <v>68</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>69</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="E34" s="0" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1014,13 +1034,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>71</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="E35" s="0" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1028,13 +1048,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>73</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1042,13 +1062,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>75</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1056,13 +1076,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>78</v>
+        <v>76</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>35</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="E38" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1070,13 +1090,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="E39" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1084,422 +1104,545 @@
         <v>39</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>80</v>
+        <v>78</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="E40" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
         <v>40</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="F41" s="0" t="s">
-        <v>18</v>
+        <v>79</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="E42" s="0" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>86</v>
+        <v>82</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="E43" s="0" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>88</v>
+        <v>83</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>84</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E44" s="0" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>89</v>
+        <v>85</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>86</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="E45" s="0" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>91</v>
+        <v>87</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>88</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="E46" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>93</v>
+        <v>89</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>90</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="E47" s="0" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>94</v>
+        <v>91</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>92</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="E48" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="E49" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>97</v>
+        <v>94</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>95</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="E50" s="0" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>99</v>
+        <v>96</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>97</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E51" s="0" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>100</v>
+        <v>98</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="E52" s="0" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>100</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="E53" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>103</v>
+        <v>101</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="E54" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>105</v>
+        <v>102</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>103</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="E55" s="0" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>107</v>
+        <v>104</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="E56" s="0" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>39</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="E57" s="0" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>110</v>
+        <v>106</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>107</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="E58" s="0" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>112</v>
+        <v>108</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>109</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E59" s="0" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B60" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C61" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="D60" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="E60" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="127.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="n">
-        <v>65</v>
-      </c>
-      <c r="B61" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E61" s="0" t="s">
-        <v>18</v>
+      <c r="D61" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>117</v>
+        <v>114</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>92</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="E62" s="0" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>118</v>
+        <v>115</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>116</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E63" s="0" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>119</v>
+        <v>117</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="E64" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>121</v>
+        <v>118</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>119</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="E65" s="0" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>122</v>
+        <v>120</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>8</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E66" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>123</v>
+        <v>121</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="E67" s="0" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>125</v>
+        <v>122</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="E68" s="0" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="D70" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="D71" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D72" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="D73" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D74" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D75" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="D76" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="D77" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="n">
         <v>77</v>
       </c>
-      <c r="B69" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="D69" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="E69" s="0" t="s">
-        <v>28</v>
+      <c r="B78" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="D78" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>